<commit_message>
Feature Black stim in Cond replaced with Stim
</commit_message>
<xml_diff>
--- a/2_Condition.xlsx
+++ b/2_Condition.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26327"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="40" documentId="13_ncr:1_{6285B7B2-83D9-C54A-BBCE-039ED38AAD9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C6614CB7-B3EC-1C47-B75F-5F33C6E76067}"/>
+  <xr:revisionPtr revIDLastSave="43" documentId="13_ncr:1_{6285B7B2-83D9-C54A-BBCE-039ED38AAD9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F32B5271-86E2-4B28-A88E-DDDE5B4D7EB4}"/>
   <bookViews>
-    <workbookView xWindow="12200" yWindow="1700" windowWidth="14400" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="6945" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="13">
   <si>
     <t>TrgCol</t>
   </si>
@@ -46,9 +46,6 @@
   </si>
   <si>
     <t>Sound/scream1.wav</t>
-  </si>
-  <si>
-    <t>Stimuli/black.PNG</t>
   </si>
   <si>
     <t>Sound/laugh1.wav</t>
@@ -160,10 +157,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -490,20 +483,20 @@
   <dimension ref="A1:D94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E91" sqref="E91"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C97" sqref="C97"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
   <cols>
-    <col min="1" max="1" width="20.83203125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="22.5" style="4" customWidth="1"/>
-    <col min="3" max="3" width="19.83203125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="12.5" style="4"/>
-    <col min="5" max="16384" width="8.83203125" style="4"/>
+    <col min="1" max="1" width="20.83984375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="22.47265625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="19.83984375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="12.47265625" style="4"/>
+    <col min="5" max="16384" width="8.83984375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="5" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="5" customFormat="1" ht="18.3" x14ac:dyDescent="0.7">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
@@ -517,12 +510,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A2" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>4</v>
@@ -531,12 +524,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A3" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>4</v>
@@ -545,12 +538,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A4" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>4</v>
@@ -559,12 +552,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A5" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>4</v>
@@ -573,12 +566,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A6" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>4</v>
@@ -587,12 +580,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A7" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>4</v>
@@ -601,12 +594,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A8" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>5</v>
@@ -615,12 +608,12 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A9" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>5</v>
@@ -629,12 +622,12 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A10" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>5</v>
@@ -643,12 +636,12 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="11" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A11" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>5</v>
@@ -657,12 +650,12 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="12" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A12" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>5</v>
@@ -671,12 +664,12 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="13" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A13" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>5</v>
@@ -685,12 +678,12 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="14" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A14" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>5</v>
@@ -699,12 +692,12 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="15" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A15" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>5</v>
@@ -713,12 +706,12 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="16" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A16" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>5</v>
@@ -727,12 +720,12 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="17" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A17" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>5</v>
@@ -741,12 +734,12 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="18" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A18" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>5</v>
@@ -755,12 +748,12 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="19" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A19" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>5</v>
@@ -769,12 +762,12 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="20" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A20" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>5</v>
@@ -783,12 +776,12 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="21" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A21" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>5</v>
@@ -797,12 +790,12 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="22" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A22" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>5</v>
@@ -811,12 +804,12 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="23" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A23" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>5</v>
@@ -825,12 +818,12 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="24" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A24" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>5</v>
@@ -839,12 +832,12 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="25" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A25" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>5</v>
@@ -853,12 +846,12 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="26" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A26" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>5</v>
@@ -867,12 +860,12 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="27" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A27" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>5</v>
@@ -881,12 +874,12 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="28" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A28" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>5</v>
@@ -895,12 +888,12 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="29" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A29" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>5</v>
@@ -909,12 +902,12 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="30" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A30" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>5</v>
@@ -923,12 +916,12 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="31" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A31" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>5</v>
@@ -937,12 +930,12 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A32" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>4</v>
@@ -951,12 +944,12 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A33" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>4</v>
@@ -965,12 +958,12 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A34" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>4</v>
@@ -979,12 +972,12 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A35" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>4</v>
@@ -993,12 +986,12 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A36" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>4</v>
@@ -1007,12 +1000,12 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A37" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>4</v>
@@ -1021,12 +1014,12 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A38" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>4</v>
@@ -1035,12 +1028,12 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A39" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>4</v>
@@ -1049,12 +1042,12 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A40" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>4</v>
@@ -1063,12 +1056,12 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A41" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>4</v>
@@ -1077,12 +1070,12 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A42" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>4</v>
@@ -1091,12 +1084,12 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A43" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>4</v>
@@ -1105,12 +1098,12 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A44" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>4</v>
@@ -1119,12 +1112,12 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A45" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>4</v>
@@ -1133,12 +1126,12 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A46" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>4</v>
@@ -1147,12 +1140,12 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A47" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>4</v>
@@ -1161,12 +1154,12 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A48" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C48" s="4" t="s">
         <v>4</v>
@@ -1175,12 +1168,12 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A49" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C49" s="4" t="s">
         <v>4</v>
@@ -1189,12 +1182,12 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A50" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C50" s="4" t="s">
         <v>4</v>
@@ -1203,12 +1196,12 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A51" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C51" s="4" t="s">
         <v>4</v>
@@ -1217,12 +1210,12 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A52" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C52" s="4" t="s">
         <v>4</v>
@@ -1231,12 +1224,12 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A53" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>4</v>
@@ -1245,12 +1238,12 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A54" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C54" s="4" t="s">
         <v>4</v>
@@ -1259,12 +1252,12 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A55" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C55" s="4" t="s">
         <v>4</v>
@@ -1273,12 +1266,12 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A56" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C56" s="4" t="s">
         <v>4</v>
@@ -1287,12 +1280,12 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A57" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C57" s="4" t="s">
         <v>4</v>
@@ -1301,12 +1294,12 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A58" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C58" s="4" t="s">
         <v>4</v>
@@ -1315,12 +1308,12 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A59" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C59" s="4" t="s">
         <v>4</v>
@@ -1329,12 +1322,12 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A60" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C60" s="4" t="s">
         <v>4</v>
@@ -1343,12 +1336,12 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A61" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C61" s="4" t="s">
         <v>4</v>
@@ -1357,12 +1350,12 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="62" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A62" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C62" s="3" t="s">
         <v>4</v>
@@ -1371,12 +1364,12 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="63" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A63" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C63" s="3" t="s">
         <v>4</v>
@@ -1385,12 +1378,12 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="64" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A64" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C64" s="3" t="s">
         <v>4</v>
@@ -1399,12 +1392,12 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="65" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A65" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C65" s="3" t="s">
         <v>4</v>
@@ -1413,12 +1406,12 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="66" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A66" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C66" s="3" t="s">
         <v>4</v>
@@ -1427,12 +1420,12 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="67" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A67" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C67" s="3" t="s">
         <v>4</v>
@@ -1441,348 +1434,348 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="68" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A68" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C68" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D68" s="1">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
+      <c r="A69" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D69" s="1">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
+      <c r="A70" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D70" s="1">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
+      <c r="A71" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D71" s="1">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
+      <c r="A72" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D72" s="1">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
+      <c r="A73" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D73" s="1">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
+      <c r="A74" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D74" s="1">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
+      <c r="A75" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D75" s="1">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
+      <c r="A76" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D76" s="1">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
+      <c r="A77" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D77" s="1">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
+      <c r="A78" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D78" s="1">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
+      <c r="A79" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D79" s="1">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
+      <c r="A80" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D80" s="1">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
+      <c r="A81" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D81" s="1">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
+      <c r="A82" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D82" s="1">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
+      <c r="A83" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D83" s="1">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
+      <c r="A84" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D84" s="1">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
+      <c r="A85" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D85" s="1">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
+      <c r="A86" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D86" s="1">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
+      <c r="A87" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D87" s="1">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
+      <c r="A88" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C88" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D88" s="1">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
+      <c r="A89" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D89" s="1">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
+      <c r="A90" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D90" s="1">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.6">
+      <c r="A91" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B91" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C91" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D91" s="1">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="A92" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D68" s="1">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B69" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C69" s="3" t="s">
+      <c r="B92" s="4" t="s">
         <v>7</v>
-      </c>
-      <c r="D69" s="1">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B70" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C70" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D70" s="1">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B71" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C71" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D71" s="1">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B72" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C72" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D72" s="1">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B73" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C73" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D73" s="1">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B74" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C74" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D74" s="1">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B75" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C75" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D75" s="1">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B76" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C76" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D76" s="1">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B77" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C77" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D77" s="1">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B78" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C78" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D78" s="1">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B79" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C79" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D79" s="1">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B80" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C80" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D80" s="1">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B81" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C81" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D81" s="1">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B82" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C82" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D82" s="1">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B83" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C83" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D83" s="1">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B84" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C84" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D84" s="1">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B85" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C85" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D85" s="1">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B86" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C86" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D86" s="1">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B87" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C87" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D87" s="1">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B88" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C88" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D88" s="1">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B89" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C89" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D89" s="1">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B90" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C90" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D90" s="1">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B91" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C91" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D91" s="1">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A92" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B92" s="4" t="s">
-        <v>6</v>
       </c>
       <c r="C92" s="4" t="s">
         <v>4</v>
@@ -1791,12 +1784,12 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A93" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C93" s="4" t="s">
         <v>4</v>
@@ -1805,12 +1798,12 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A94" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C94" s="4" t="s">
         <v>4</v>
@@ -2009,18 +2002,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2042,6 +2035,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4BCAEFB8-08FC-4F45-B367-68A06CA5E545}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F795CB29-6365-4DA8-8C2F-885C5D31C81A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="64b0b0ad-49a7-4b34-8eba-9a240439451d"/>
@@ -2055,12 +2056,4 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4BCAEFB8-08FC-4F45-B367-68A06CA5E545}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
FEATURE Added Space press for Trigg, had to add black stim in Cond for UCS after Trig
</commit_message>
<xml_diff>
--- a/2_Condition.xlsx
+++ b/2_Condition.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26327"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="43" documentId="13_ncr:1_{6285B7B2-83D9-C54A-BBCE-039ED38AAD9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F32B5271-86E2-4B28-A88E-DDDE5B4D7EB4}"/>
+  <xr:revisionPtr revIDLastSave="49" documentId="13_ncr:1_{6285B7B2-83D9-C54A-BBCE-039ED38AAD9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2233EFBE-7B21-4D17-9A9D-C1CCA7BEF8DB}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="6945" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="20928" windowHeight="13152" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="14">
   <si>
     <t>TrgCol</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>Stimuli/Pos_UCS.BMP</t>
+  </si>
+  <si>
+    <t>Stimuli/Raw_black.BMP</t>
   </si>
 </sst>
 </file>
@@ -157,6 +160,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -483,8 +490,8 @@
   <dimension ref="A1:D94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C97" sqref="C97"/>
+      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B98" sqref="B98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
@@ -1775,7 +1782,7 @@
         <v>7</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C92" s="4" t="s">
         <v>4</v>
@@ -1789,7 +1796,7 @@
         <v>7</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C93" s="4" t="s">
         <v>4</v>
@@ -1803,7 +1810,7 @@
         <v>7</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C94" s="4" t="s">
         <v>4</v>
@@ -1818,6 +1825,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DCC15C826F9CD04C984C1E59D79D0BF3" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4323ffbe69f4456b442358682c62cfba">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="64b0b0ad-49a7-4b34-8eba-9a240439451d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="94ec3c4b7e8ae219eb184f3ca94c286d" ns2:_="">
     <xsd:import namespace="64b0b0ad-49a7-4b34-8eba-9a240439451d"/>
@@ -2001,22 +2023,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F795CB29-6365-4DA8-8C2F-885C5D31C81A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="64b0b0ad-49a7-4b34-8eba-9a240439451d"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4BCAEFB8-08FC-4F45-B367-68A06CA5E545}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{899E66D0-C9AE-42BF-A4B6-2A0DE66F65C9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2032,28 +2063,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4BCAEFB8-08FC-4F45-B367-68A06CA5E545}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F795CB29-6365-4DA8-8C2F-885C5D31C81A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="64b0b0ad-49a7-4b34-8eba-9a240439451d"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>